<commit_message>
updated figures for revisions
</commit_message>
<xml_diff>
--- a/tables/TableS1_emissions_scenarios.xlsx
+++ b/tables/TableS1_emissions_scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/aquacast/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F087D8-C1E7-F844-8FA0-E9A9FFDA5E2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827AA5F7-5FBC-DE49-9E29-6BFFB3CBCD0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="4140" windowWidth="25440" windowHeight="15000" xr2:uid="{D45F6DD9-3AE0-1442-8297-5BFD33B521B3}"/>
+    <workbookView xWindow="6360" yWindow="6960" windowWidth="25440" windowHeight="15000" xr2:uid="{D45F6DD9-3AE0-1442-8297-5BFD33B521B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Scenario</t>
   </si>
@@ -270,6 +270,21 @@
       </rPr>
       <t> eq) at stabilization after 2100</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">bcc-csm1-1, bcc-csm1-1-m, CanESM2, CCSM4, CESM1-CAM5, CNRM-CM5, CSIRO-Mk3-6-0, EC-EARTH, FIO-ESM, GFDL-CM3, GFDL-ESM2G, GFDL- ESM2M, GISS-E2-H, GISS-E2-H, GISS-E2-H, GISS-E2-R, GISS-E2-R, GISS- E2-R, HadGEM2-AO, HadGEM2-ES, IPSL-CM5A-LR, IPSL-CM5A-MR, MIROC5, MPI-ESM-LR, MPI-ESM-MR </t>
+  </si>
+  <si>
+    <t>ACCESS1-0, ACCESS1-3, bcc-csm1-1, bcc-csm1-1-m, CanESM2, CCSM4, CESM1-BGC, CESM1-CAM5, CMCC-CM, CMCC-CMS, CNRM-CM5, CSIRO- Mk3-6-0, EC-EARTH, FIO-ESM, GFDL-CM3, GFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcc-csm1-1-m, CCSM4, CESM1-CAM5, CSIRO-Mk3-6-0, FIO-ESM, GFDL- CM3, GFDL-ESM2G, GFDL-ESM2M, GISS-E2-H, GISS-E2-H, GISS-E2-H, GISS-E2-R, GISS-E2-R, GISS-E2-R, HadGEM2-AO, HadGEM2-ES, IPSL- CM5A-LR, MIROC5, MRI-CGCM3, NorESM1-M, NorESM1-ME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCESS1-0, ACCESS1-3, bcc-csm1-1, CanESM2, CCSM4, CESM1-BGC, CESM1-CAM5, CMCC-CM, CMCC-CMS, CNRM-CM5, CSIRO-Mk3-6-0, EC- EARTH, FIO-ESM, GFDL-CM3, GFDL-ESM2G, GFDL-ESM2M, GISS-E2-H, GISS-E2-H, GISS-E2-H, GISS-E2-R, GISS-E2-R, GISS-E2-R, HadGEM2-CC, HadGEM2-ES, inmcm4, IPSL-CM5A-LR, IPSL-CM5A-MR, IPSL-CM5B-LR, MIROC5, MPI-ESM-LR, MPI-ESM-MR, MRI-CGCM3, NorESM1-M, NorESM1-ME </t>
+  </si>
+  <si>
+    <t>ESM ensembled for the Free et al. (2020) fisheries analysis</t>
   </si>
 </sst>
 </file>
@@ -336,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -347,6 +362,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -662,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD2C0E7-95AA-DE41-AFB0-19847F71DBAB}">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -673,10 +691,11 @@
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18" thickBot="1">
+    <row r="2" spans="1:5" ht="18" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -689,8 +708,11 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="42" thickTop="1">
+    <row r="3" spans="1:5" ht="103" thickTop="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -703,8 +725,11 @@
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="40">
+    <row r="4" spans="1:5" ht="68">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -717,8 +742,11 @@
       <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="39">
+    <row r="5" spans="1:5" ht="85">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -731,8 +759,11 @@
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="39">
+    <row r="6" spans="1:5" ht="136">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -745,18 +776,22 @@
       <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E6" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>